<commit_message>
Avaliação de força de maré e escolha de melhor código//Inicio de criação de .exe//Criação de ícone de cliente
</commit_message>
<xml_diff>
--- a/GRARED_P_exemplo.xlsx
+++ b/GRARED_P_exemplo.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -191,6 +191,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="justify" readingOrder="1"/>
     </xf>
@@ -218,8 +220,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,8 +523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N1" sqref="A1:N2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,38 +552,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="13" t="s">
+      <c r="C1" s="21"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="14"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="14" t="s">
+      <c r="F1" s="16"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="14"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="11" t="s">
+      <c r="I1" s="16"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="L1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="14"/>
-      <c r="N1" s="11" t="s">
+      <c r="M1" s="16"/>
+      <c r="N1" s="13" t="s">
         <v>4</v>
       </c>
       <c r="O1" s="8"/>
     </row>
     <row r="2" spans="1:15" s="2" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17"/>
+      <c r="A2" s="19"/>
       <c r="B2" s="9">
         <v>1</v>
       </c>
@@ -611,14 +611,14 @@
       <c r="J2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="12"/>
+      <c r="K2" s="14"/>
       <c r="L2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="12"/>
+      <c r="N2" s="14"/>
       <c r="O2" s="8"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -635,19 +635,19 @@
         <v>2333.5700000000002</v>
       </c>
       <c r="E3" s="5">
-        <v>-22</v>
+        <v>-23</v>
       </c>
       <c r="F3" s="5">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="G3" s="1">
         <v>23.34</v>
       </c>
       <c r="H3" s="5">
-        <v>-110</v>
+        <v>-46</v>
       </c>
       <c r="I3" s="5">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="J3" s="1">
         <v>12.23</v>
@@ -656,10 +656,10 @@
         <v>2.3330000000000002</v>
       </c>
       <c r="L3" s="5">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="M3" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="N3" s="4">
         <v>23.565999999999999</v>
@@ -679,19 +679,19 @@
         <v>2552.0100000000002</v>
       </c>
       <c r="E4" s="5">
-        <v>-22</v>
+        <v>-23</v>
       </c>
       <c r="F4" s="5">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="G4" s="1">
         <v>24.23</v>
       </c>
       <c r="H4" s="5">
-        <v>-110</v>
+        <v>-46</v>
       </c>
       <c r="I4" s="5">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="J4" s="1">
         <v>14.45</v>
@@ -700,10 +700,10 @@
         <v>1.89</v>
       </c>
       <c r="L4" s="5">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="M4" s="1">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="N4" s="4">
         <v>23.677</v>
@@ -723,19 +723,19 @@
         <v>2770.45</v>
       </c>
       <c r="E5" s="5">
-        <v>-22</v>
+        <v>-23</v>
       </c>
       <c r="F5" s="5">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="G5" s="1">
         <v>25.12</v>
       </c>
       <c r="H5" s="5">
-        <v>-110</v>
+        <v>-46</v>
       </c>
       <c r="I5" s="5">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="J5" s="1">
         <v>16.670000000000002</v>
@@ -744,10 +744,10 @@
         <v>1.4470000000000001</v>
       </c>
       <c r="L5" s="5">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="M5" s="1">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="N5" s="4">
         <v>23.788</v>
@@ -767,19 +767,19 @@
         <v>2988.89</v>
       </c>
       <c r="E6" s="5">
-        <v>-22</v>
+        <v>-23</v>
       </c>
       <c r="F6" s="5">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="G6" s="1">
         <v>26.01</v>
       </c>
       <c r="H6" s="5">
-        <v>-110</v>
+        <v>-46</v>
       </c>
       <c r="I6" s="5">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="J6" s="1">
         <v>18.89</v>
@@ -788,10 +788,10 @@
         <v>1.004</v>
       </c>
       <c r="L6" s="5">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="M6" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N6" s="4">
         <v>23.899000000000001</v>
@@ -811,19 +811,19 @@
         <v>3207.33</v>
       </c>
       <c r="E7" s="5">
-        <v>-22</v>
+        <v>-23</v>
       </c>
       <c r="F7" s="5">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="G7" s="1">
         <v>26.9</v>
       </c>
       <c r="H7" s="5">
-        <v>-110</v>
+        <v>-46</v>
       </c>
       <c r="I7" s="5">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="J7" s="1">
         <v>21.11</v>
@@ -832,10 +832,10 @@
         <v>0.56100000000000005</v>
       </c>
       <c r="L7" s="5">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="M7" s="1">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="N7" s="4">
         <v>24.01</v>
@@ -855,19 +855,19 @@
         <v>2991.25</v>
       </c>
       <c r="E8" s="5">
-        <v>-22</v>
+        <v>-23</v>
       </c>
       <c r="F8" s="5">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="G8" s="1">
         <v>26.06</v>
       </c>
       <c r="H8" s="5">
-        <v>-110</v>
+        <v>-46</v>
       </c>
       <c r="I8" s="5">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="J8" s="1">
         <v>19.010000000000002</v>
@@ -876,10 +876,10 @@
         <v>0.98699999999999999</v>
       </c>
       <c r="L8" s="5">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="M8" s="1">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="N8" s="4">
         <v>23.989000000000001</v>
@@ -899,19 +899,19 @@
         <v>2775.17</v>
       </c>
       <c r="E9" s="5">
-        <v>-22</v>
+        <v>-23</v>
       </c>
       <c r="F9" s="5">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="G9" s="1">
         <v>25.22</v>
       </c>
       <c r="H9" s="5">
-        <v>-110</v>
+        <v>-46</v>
       </c>
       <c r="I9" s="5">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="J9" s="1">
         <v>16.91</v>
@@ -920,10 +920,10 @@
         <v>1.413</v>
       </c>
       <c r="L9" s="5">
+        <v>21</v>
+      </c>
+      <c r="M9" s="1">
         <v>14</v>
-      </c>
-      <c r="M9" s="1">
-        <v>22</v>
       </c>
       <c r="N9" s="4">
         <v>23.968</v>
@@ -943,19 +943,19 @@
         <v>2559.09</v>
       </c>
       <c r="E10" s="5">
-        <v>-22</v>
+        <v>-23</v>
       </c>
       <c r="F10" s="5">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="G10" s="1">
         <v>24.38</v>
       </c>
       <c r="H10" s="5">
-        <v>-110</v>
+        <v>-46</v>
       </c>
       <c r="I10" s="5">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="J10" s="1">
         <v>14.81</v>
@@ -964,10 +964,10 @@
         <v>1.839</v>
       </c>
       <c r="L10" s="5">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="M10" s="1">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="N10" s="4">
         <v>23.946999999999999</v>
@@ -987,19 +987,19 @@
         <v>2343.0100000000002</v>
       </c>
       <c r="E11" s="5">
-        <v>-22</v>
+        <v>-23</v>
       </c>
       <c r="F11" s="5">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="G11" s="1">
         <v>23.54</v>
       </c>
       <c r="H11" s="5">
-        <v>-110</v>
+        <v>-46</v>
       </c>
       <c r="I11" s="5">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="J11" s="1">
         <v>12.71</v>
@@ -1008,10 +1008,10 @@
         <v>2.2650000000000001</v>
       </c>
       <c r="L11" s="5">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="M11" s="1">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="N11" s="4">
         <v>23.925999999999998</v>
@@ -1031,19 +1031,19 @@
         <v>2126.9299999999998</v>
       </c>
       <c r="E12" s="5">
-        <v>-22</v>
+        <v>-23</v>
       </c>
       <c r="F12" s="5">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="G12" s="1">
         <v>23.34</v>
       </c>
       <c r="H12" s="5">
-        <v>-110</v>
+        <v>-46</v>
       </c>
       <c r="I12" s="5">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="J12" s="1">
         <v>12.23</v>
@@ -1052,10 +1052,10 @@
         <v>2.3330000000000002</v>
       </c>
       <c r="L12" s="5">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="M12" s="1">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="N12" s="4">
         <v>23.565999999999999</v>
@@ -1080,48 +1080,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2002"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q1992" sqref="Q1992"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.140625" style="21"/>
-    <col min="4" max="4" width="9.140625" style="20"/>
+    <col min="3" max="3" width="9.140625" style="12"/>
+    <col min="4" max="4" width="9.140625" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="13" t="s">
+      <c r="C1" s="21"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="14"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="14" t="s">
+      <c r="F1" s="16"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="14"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="11" t="s">
+      <c r="I1" s="16"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="L1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="14"/>
-      <c r="N1" s="11" t="s">
+      <c r="M1" s="16"/>
+      <c r="N1" s="13" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17"/>
+      <c r="A2" s="19"/>
       <c r="B2" s="9">
         <v>1</v>
       </c>
@@ -1149,14 +1149,14 @@
       <c r="J2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="12"/>
+      <c r="K2" s="14"/>
       <c r="L2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="12"/>
+      <c r="N2" s="14"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1">

</xml_diff>